<commit_message>
AFE master bom itt, layout itt, sch itt
</commit_message>
<xml_diff>
--- a/BMS_doc/AFE_MASTER_BOM.xlsx
+++ b/BMS_doc/AFE_MASTER_BOM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Green_Fuel\GF_BMS\BMS_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-KIT33771A-SPI_EVB_0424" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="257">
   <si>
     <t>Item</t>
   </si>
@@ -252,9 +252,6 @@
     <t>C22, C76</t>
   </si>
   <si>
-    <t>R79, R87, R88, R96, R105, R106</t>
-  </si>
-  <si>
     <t>R15, R16, R17, R18, R19, R20, R21, R44, R45, R50, R51, R52, R53, R54, R55</t>
   </si>
   <si>
@@ -492,12 +489,6 @@
     <t>CRCW06032R00FKEAHP</t>
   </si>
   <si>
-    <t>R31,R95,R97,R87,R88,R96,R105,R106</t>
-  </si>
-  <si>
-    <t>127E</t>
-  </si>
-  <si>
     <t>R83</t>
   </si>
   <si>
@@ -796,6 +787,9 @@
   </si>
   <si>
     <t>GF_AFE board Revised: Sunday, OCT 14, 2018</t>
+  </si>
+  <si>
+    <t>R79, R87, R88, R96, R105, R106,R31,R95,R97,R87,R88,R96,R105,R106,R119</t>
   </si>
 </sst>
 </file>
@@ -1717,11 +1711,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,7 +1734,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1901,7 +1895,7 @@
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>28</v>
@@ -1982,10 +1976,10 @@
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>127</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>128</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>43</v>
@@ -2005,11 +1999,11 @@
         <v>9</v>
       </c>
       <c r="B12" s="5">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="14" t="s">
-        <v>77</v>
+        <v>256</v>
       </c>
       <c r="E12" s="12">
         <v>127</v>
@@ -2036,7 +2030,7 @@
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>51</v>
@@ -2063,7 +2057,7 @@
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>54</v>
@@ -2090,7 +2084,7 @@
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>57</v>
@@ -2117,7 +2111,7 @@
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>60</v>
@@ -2143,7 +2137,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>38</v>
@@ -2169,13 +2163,13 @@
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2186,13 +2180,13 @@
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2203,13 +2197,13 @@
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="J20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2220,13 +2214,13 @@
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="J21" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2237,10 +2231,10 @@
         <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>64</v>
@@ -2263,7 +2257,7 @@
         <v>4</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>66</v>
@@ -2289,13 +2283,13 @@
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -2306,22 +2300,22 @@
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E25" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="H25" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="I25" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="J25" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2332,22 +2326,22 @@
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="H26" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="I26" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="I26" s="8" t="s">
-        <v>107</v>
-      </c>
       <c r="J26" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2358,22 +2352,22 @@
         <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="H27" s="8" t="s">
+      <c r="I27" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="I27" s="8" t="s">
-        <v>111</v>
-      </c>
       <c r="J27" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2384,22 +2378,22 @@
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F28" s="8" t="s">
+      <c r="H28" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="I28" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="J28" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2410,22 +2404,22 @@
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="H29" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="I29" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="I29" s="8" t="s">
-        <v>123</v>
-      </c>
       <c r="J29" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2436,19 +2430,19 @@
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>124</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>125</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>48</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J30" s="8" t="s">
         <v>50</v>
@@ -2462,19 +2456,19 @@
         <v>7</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>132</v>
       </c>
       <c r="H31" s="8" t="s">
         <v>27</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J31" s="8" t="s">
         <v>18</v>
@@ -2488,22 +2482,22 @@
         <v>2</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="H32" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="I32" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="I32" s="8" t="s">
-        <v>138</v>
-      </c>
       <c r="J32" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2514,22 +2508,22 @@
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="H33" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="I33" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="I33" s="8" t="s">
-        <v>144</v>
-      </c>
       <c r="J33" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2540,25 +2534,25 @@
         <v>1</v>
       </c>
       <c r="C34" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="H34" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="I34" s="8" t="s">
-        <v>150</v>
-      </c>
       <c r="J34" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2569,10 +2563,10 @@
         <v>4</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2583,105 +2577,105 @@
         <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="H36" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="I36" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="H36" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>156</v>
-      </c>
       <c r="J36" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="F37" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="H37" s="8" t="s">
-        <v>48</v>
+        <v>159</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>50</v>
+        <v>160</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B38" s="2">
         <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B39" s="2">
         <v>1</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>165</v>
+        <v>35</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>168</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40" s="2">
         <v>1</v>
@@ -2690,559 +2684,533 @@
         <v>169</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F40" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="I40" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="8" t="s">
         <v>173</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>12</v>
+        <v>178</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>178</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B43" s="2">
         <v>1</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="H43" s="8" t="s">
         <v>181</v>
-      </c>
-      <c r="I43" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44" s="2">
         <v>1</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B45" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B46" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B47" s="2">
         <v>1</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B48" s="2">
         <v>1</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="8" t="s">
         <v>192</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B49" s="2">
         <v>1</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F49" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="H49" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="I49" s="8" t="s">
-        <v>196</v>
-      </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B50" s="2">
         <v>1</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>197</v>
       </c>
+      <c r="F50" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B51" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F51" s="8" t="s">
         <v>201</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I51" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B52" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B53" s="2">
         <v>3</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>204</v>
       </c>
+      <c r="F53" s="8" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B54" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D54" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B55" s="2">
         <v>1</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B56" s="2">
         <v>1</v>
       </c>
       <c r="D56" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B57" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E57" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="8" t="s">
         <v>213</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="I57" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="J57" s="8" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B58" s="2">
         <v>3</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E58" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="F58" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="H58" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="J58" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="H58" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="I58" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="J58" s="8" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B59" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="H59" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="J59" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B60" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D60" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B61" s="2">
         <v>2</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B62" s="2">
         <v>2</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B63" s="2">
         <v>2</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B64" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D64" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="I64" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>227</v>
+      <c r="J64" s="8" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B65" s="2">
         <v>1</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="J65" s="8" t="s">
-        <v>233</v>
+        <v>235</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B66" s="2">
         <v>1</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F66" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="H66" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="I66" s="8" t="s">
         <v>238</v>
-      </c>
-      <c r="J66" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B67" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D67" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B68" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D68" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B69" s="2">
-        <v>3</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>244</v>
+        <v>6</v>
+      </c>
+      <c r="D69" s="16" t="s">
+        <v>246</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B70" s="2">
         <v>6</v>
       </c>
-      <c r="D70" s="16" t="s">
-        <v>249</v>
+      <c r="D70" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
-        <v>68</v>
-      </c>
-      <c r="B71" s="2">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D72" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E72" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="5">
-        <v>70</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -3252,33 +3220,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c4672b8b-43e2-4139-8cd1-27ad03f081e7">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <dd399bed73eb4e21ba4b4b5eeb50a8b4 xmlns="c4672b8b-43e2-4139-8cd1-27ad03f081e7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">fba6ddd2-c0d6-406a-843f-19fb8f95d116</TermId>
-        </TermInfo>
-      </Terms>
-    </dd399bed73eb4e21ba4b4b5eeb50a8b4>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100365B9D8916E0C148AAD2A59EF921597E" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d9331e4b492c85a6adb8400544173777">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c4672b8b-43e2-4139-8cd1-27ad03f081e7" xmlns:ns3="f8cd1e16-0731-4200-9ee6-df6e2184771e" xmlns:ns4="1f7e2bd1-5fdf-4d6b-8b99-ef650a991a33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="68e0f9790db2f35a3add71fa64d56bef" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="c4672b8b-43e2-4139-8cd1-27ad03f081e7"/>
@@ -3482,25 +3423,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{817A1FC8-D3A3-4B4B-9419-3DB2734E9FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c4672b8b-43e2-4139-8cd1-27ad03f081e7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFEF643C-744E-47E4-BE01-550303BDE769}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c4672b8b-43e2-4139-8cd1-27ad03f081e7">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <dd399bed73eb4e21ba4b4b5eeb50a8b4 xmlns="c4672b8b-43e2-4139-8cd1-27ad03f081e7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">fba6ddd2-c0d6-406a-843f-19fb8f95d116</TermId>
+        </TermInfo>
+      </Terms>
+    </dd399bed73eb4e21ba4b4b5eeb50a8b4>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2403EAF2-654B-490C-A2E2-A6A3E009296C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3518,4 +3468,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFEF643C-744E-47E4-BE01-550303BDE769}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{817A1FC8-D3A3-4B4B-9419-3DB2734E9FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c4672b8b-43e2-4139-8cd1-27ad03f081e7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
afe master bom ediited
</commit_message>
<xml_diff>
--- a/BMS_doc/AFE_MASTER_BOM.xlsx
+++ b/BMS_doc/AFE_MASTER_BOM.xlsx
@@ -1714,8 +1714,8 @@
   <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37:XFD37"/>
+      <pane ySplit="3" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3195,6 +3195,9 @@
       <c r="A71" s="5">
         <v>69</v>
       </c>
+      <c r="B71" s="2">
+        <v>1</v>
+      </c>
       <c r="D71" s="1" t="s">
         <v>251</v>
       </c>
@@ -3205,6 +3208,9 @@
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>70</v>
+      </c>
+      <c r="B72" s="2">
+        <v>1</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>253</v>

</xml_diff>